<commit_message>
fix error from receitps manage
</commit_message>
<xml_diff>
--- a/document/co_so_du_lieu_nhom_31.xlsx
+++ b/document/co_so_du_lieu_nhom_31.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\Work\Đồ án\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\J2School-main\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD7031A-56BA-438D-BA5D-C920184C00F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB67240C-53CF-426B-80DA-8FFF0B6B45D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="960" windowWidth="16584" windowHeight="10956" xr2:uid="{74463A8A-8549-43CD-9702-C9EAFB65584C}"/>
+    <workbookView xWindow="10080" yWindow="768" windowWidth="16584" windowHeight="10956" xr2:uid="{74463A8A-8549-43CD-9702-C9EAFB65584C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>manufacturers</t>
   </si>
@@ -93,6 +93,12 @@
     <t>customer_id </t>
   </si>
   <si>
+    <t>product_id </t>
+  </si>
+  <si>
+    <t>carts</t>
+  </si>
+  <si>
     <t>admins</t>
   </si>
   <si>
@@ -120,26 +126,14 @@
     <t>receiver_address</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>dob</t>
-  </si>
-  <si>
-    <t>receipt_id</t>
-  </si>
-  <si>
-    <t>receipt_detail</t>
-  </si>
-  <si>
-    <t>product_id</t>
+    <t>note</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,14 +185,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -221,14 +207,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -544,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9351AF5D-E696-4F88-B233-01071196C1CA}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,7 +596,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -630,58 +615,62 @@
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>30</v>
+      <c r="A10" t="s">
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -689,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -697,7 +686,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -705,24 +694,11 @@
         <v>16</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="E18" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="E19" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>